<commit_message>
Added Sankey and Rebalancing app
</commit_message>
<xml_diff>
--- a/assets/Historical Performance.xlsx
+++ b/assets/Historical Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard\PycharmProjects\dash\YT_Dash_Tutorial\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5D50E0-7C86-496C-A70A-047DED59CEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7D3A27-DD8C-46AC-A14C-4AD9A340E069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="990" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="240" windowWidth="29040" windowHeight="16455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="101">
   <si>
     <t>Ticker</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>Yesterday Close</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>WMT</t>
   </si>
   <si>
-    <t>Consumer Stales</t>
-  </si>
-  <si>
     <t>Hypermarkets &amp; Super Centres</t>
   </si>
   <si>
@@ -337,13 +331,20 @@
   </si>
   <si>
     <t>American Tower Corp</t>
+  </si>
+  <si>
+    <t>Consumer Staples</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +356,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -400,10 +408,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -411,8 +420,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -713,15 +726,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -755,1112 +775,1050 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M1" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
-      <c r="G2">
+      <c r="F2" s="4">
         <v>3518.099975585938</v>
       </c>
-      <c r="H2">
+      <c r="G2" s="4">
         <v>3250</v>
       </c>
-      <c r="I2">
+      <c r="H2" s="4">
         <v>3118.099975585938</v>
       </c>
-      <c r="J2">
+      <c r="I2" s="4">
         <v>2838.800048828125</v>
       </c>
-      <c r="K2">
+      <c r="J2" s="4">
         <v>3237.7999877929692</v>
       </c>
+      <c r="K2" s="4">
+        <v>3049.500122070312</v>
+      </c>
       <c r="L2">
-        <v>3049.500122070312</v>
-      </c>
-      <c r="M2">
         <v>1904.400024414062</v>
       </c>
-      <c r="N2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3">
-        <v>9</v>
-      </c>
-      <c r="G3">
+      <c r="F3" s="4">
         <v>2434.409912109375</v>
       </c>
-      <c r="H3">
+      <c r="G3" s="4">
         <v>2602.079956054688</v>
       </c>
-      <c r="I3">
+      <c r="H3" s="4">
         <v>2595.7933044433589</v>
       </c>
-      <c r="J3">
+      <c r="I3" s="4">
         <v>2695.3525085449219</v>
       </c>
-      <c r="K3">
+      <c r="J3" s="4">
         <v>2344.502197265625</v>
       </c>
+      <c r="K3" s="4">
+        <v>2537.4248657226558</v>
+      </c>
       <c r="L3">
-        <v>2537.4248657226558</v>
-      </c>
-      <c r="M3">
         <v>1921.855819702148</v>
       </c>
-      <c r="N3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4">
+      <c r="F4" s="4">
         <v>11203.3203125</v>
       </c>
-      <c r="H4">
+      <c r="G4" s="4">
         <v>10722.7998046875</v>
       </c>
-      <c r="I4">
+      <c r="H4" s="4">
         <v>9800</v>
       </c>
-      <c r="J4">
+      <c r="I4" s="4">
         <v>9451.48046875</v>
       </c>
-      <c r="K4">
+      <c r="J4" s="4">
         <v>8335.240234375</v>
       </c>
+      <c r="K4" s="4">
+        <v>6340.60009765625</v>
+      </c>
       <c r="L4">
-        <v>6340.60009765625</v>
-      </c>
-      <c r="M4">
         <v>4684.72021484375</v>
       </c>
-      <c r="N4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
       <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5">
+        <v>22</v>
+      </c>
+      <c r="F5" s="4">
         <v>13063.48046875</v>
       </c>
-      <c r="H5">
+      <c r="G5" s="4">
         <v>14799.2802734375</v>
       </c>
-      <c r="I5">
+      <c r="H5" s="4">
         <v>13796.3203125</v>
       </c>
-      <c r="J5">
+      <c r="I5" s="4">
         <v>13036.2001953125</v>
       </c>
-      <c r="K5">
+      <c r="J5" s="4">
         <v>12638.1201171875</v>
       </c>
+      <c r="K5" s="4">
+        <v>13229.83984375</v>
+      </c>
       <c r="L5">
-        <v>13229.83984375</v>
-      </c>
-      <c r="M5">
         <v>7075.47998046875</v>
       </c>
-      <c r="N5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
       <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6">
-        <v>43</v>
-      </c>
-      <c r="G6">
+        <v>18</v>
+      </c>
+      <c r="F6" s="4">
         <v>6437.5302886962891</v>
       </c>
-      <c r="H6">
+      <c r="G6" s="4">
         <v>6396.9861755371094</v>
       </c>
-      <c r="I6">
+      <c r="H6" s="4">
         <v>5728.0480041503906</v>
       </c>
-      <c r="J6">
+      <c r="I6" s="4">
         <v>5448.5368499755859</v>
       </c>
-      <c r="K6">
+      <c r="J6" s="4">
         <v>5372.8600387573242</v>
       </c>
+      <c r="K6" s="4">
+        <v>5377.2866058349609</v>
+      </c>
       <c r="L6">
-        <v>5377.2866058349609</v>
-      </c>
-      <c r="M6">
         <v>2183.9131202697749</v>
       </c>
-      <c r="N6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>31</v>
       </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7">
-        <v>44</v>
-      </c>
-      <c r="G7">
+      <c r="F7" s="5">
         <v>4800.3999328613281</v>
       </c>
-      <c r="H7">
+      <c r="G7" s="4">
         <v>5071</v>
       </c>
-      <c r="I7">
+      <c r="H7" s="4">
         <v>4920.0799865722656</v>
       </c>
-      <c r="J7">
+      <c r="I7" s="4">
         <v>4579.0799865722656</v>
       </c>
-      <c r="K7">
+      <c r="J7" s="4">
         <v>5481.5200805664063</v>
       </c>
+      <c r="K7" s="4">
+        <v>3295.1599731445308</v>
+      </c>
       <c r="L7">
-        <v>3295.1599731445308</v>
-      </c>
-      <c r="M7">
         <v>2218.4799194335942</v>
       </c>
-      <c r="N7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
-      </c>
       <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8">
-        <v>10</v>
-      </c>
-      <c r="G8">
+        <v>22</v>
+      </c>
+      <c r="F8" s="4">
         <v>2908.900146484375</v>
       </c>
-      <c r="H8">
+      <c r="G8" s="4">
         <v>3057.6998901367192</v>
       </c>
-      <c r="I8">
+      <c r="H8" s="4">
         <v>2767.2000122070308</v>
       </c>
-      <c r="J8">
+      <c r="I8" s="4">
         <v>1956.799926757812</v>
       </c>
-      <c r="K8">
+      <c r="J8" s="4">
         <v>2396.6000366210942</v>
       </c>
+      <c r="K8" s="4">
+        <v>2044.9000549316411</v>
+      </c>
       <c r="L8">
-        <v>2044.9000549316411</v>
-      </c>
-      <c r="M8">
         <v>452.29999542236328</v>
       </c>
-      <c r="N8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>36</v>
-      </c>
       <c r="E9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9">
-        <v>47</v>
-      </c>
-      <c r="G9">
+        <v>31</v>
+      </c>
+      <c r="F9" s="5">
         <v>4435.8598709106454</v>
       </c>
-      <c r="H9">
+      <c r="G9" s="4">
         <v>4325.8800430297852</v>
       </c>
-      <c r="I9">
+      <c r="H9" s="4">
         <v>3925.9099426269531</v>
       </c>
-      <c r="J9">
+      <c r="I9" s="4">
         <v>3385.4099426269531</v>
       </c>
-      <c r="K9">
+      <c r="J9" s="4">
         <v>5187.8598709106454</v>
       </c>
+      <c r="K9" s="4">
+        <v>2145.079971313477</v>
+      </c>
       <c r="L9">
-        <v>2145.079971313477</v>
-      </c>
-      <c r="M9">
         <v>561.17998027801514</v>
       </c>
-      <c r="N9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
       <c r="E10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10">
-        <v>9</v>
-      </c>
-      <c r="G10">
+        <v>22</v>
+      </c>
+      <c r="F10" s="5">
         <v>5258.6998901367188</v>
       </c>
-      <c r="H10">
+      <c r="G10" s="4">
         <v>5763.5101318359384</v>
       </c>
-      <c r="I10">
+      <c r="H10" s="4">
         <v>5715.18017578125</v>
       </c>
-      <c r="J10">
+      <c r="I10" s="4">
         <v>5751.8074951171884</v>
       </c>
-      <c r="K10">
+      <c r="J10" s="4">
         <v>5348.3746948242188</v>
       </c>
+      <c r="K10" s="4">
+        <v>3125.0739440917969</v>
+      </c>
       <c r="L10">
-        <v>3125.0739440917969</v>
-      </c>
-      <c r="M10">
         <v>1758.3225402832029</v>
       </c>
-      <c r="N10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
-      </c>
       <c r="E11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11">
-        <v>65</v>
-      </c>
-      <c r="G11">
+        <v>22</v>
+      </c>
+      <c r="F11" s="4">
         <v>2481.0498809814449</v>
       </c>
-      <c r="H11">
+      <c r="G11" s="4">
         <v>2806.0498809814449</v>
       </c>
-      <c r="I11">
+      <c r="H11" s="4">
         <v>2954.8999404907231</v>
       </c>
-      <c r="J11">
+      <c r="I11" s="4">
         <v>2344.5499801635742</v>
       </c>
-      <c r="K11">
+      <c r="J11" s="4">
         <v>3370.900039672852</v>
       </c>
+      <c r="K11" s="4">
+        <v>973.05001735687256</v>
+      </c>
       <c r="L11">
-        <v>973.05001735687256</v>
-      </c>
-      <c r="M11">
         <v>188.50000619888311</v>
       </c>
-      <c r="N11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
         <v>41</v>
       </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
       <c r="E12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12">
-        <v>30</v>
-      </c>
-      <c r="G12">
+        <v>14</v>
+      </c>
+      <c r="F12" s="4">
         <v>7530</v>
       </c>
-      <c r="H12">
+      <c r="G12" s="4">
         <v>5800.8000183105469</v>
       </c>
-      <c r="I12">
+      <c r="H12" s="4">
         <v>5774.3998718261719</v>
       </c>
-      <c r="J12">
+      <c r="I12" s="4">
         <v>4426.5000915527344</v>
       </c>
-      <c r="K12">
+      <c r="J12" s="4">
         <v>7198.2000732421884</v>
       </c>
+      <c r="K12" s="4">
+        <v>3577.8000640869141</v>
+      </c>
       <c r="L12">
-        <v>3577.8000640869141</v>
-      </c>
-      <c r="M12">
         <v>189.2999982833862</v>
       </c>
-      <c r="N12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
       <c r="E13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13">
-        <v>65</v>
-      </c>
-      <c r="G13">
+        <v>31</v>
+      </c>
+      <c r="F13" s="4">
         <v>12453.349761962891</v>
       </c>
-      <c r="H13">
+      <c r="G13" s="4">
         <v>11020.099563598629</v>
       </c>
-      <c r="I13">
+      <c r="H13" s="4">
         <v>12528.10035705566</v>
       </c>
-      <c r="J13">
+      <c r="I13" s="4">
         <v>11451.699523925779</v>
       </c>
-      <c r="K13">
+      <c r="J13" s="4">
         <v>8192.6000595092773</v>
       </c>
+      <c r="K13" s="4">
+        <v>3900</v>
+      </c>
       <c r="L13">
-        <v>3900</v>
-      </c>
-      <c r="M13">
         <v>2594.7998809814449</v>
       </c>
-      <c r="N13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
         <v>44</v>
       </c>
-      <c r="C14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" t="s">
-        <v>45</v>
-      </c>
       <c r="E14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14">
-        <v>40</v>
-      </c>
-      <c r="G14">
+        <v>14</v>
+      </c>
+      <c r="F14" s="4">
         <v>11240.400390625</v>
       </c>
-      <c r="H14">
+      <c r="G14" s="4">
         <v>9824.7998046875</v>
       </c>
-      <c r="I14">
+      <c r="H14" s="4">
         <v>10691.19995117188</v>
       </c>
-      <c r="J14">
+      <c r="I14" s="4">
         <v>10070</v>
       </c>
-      <c r="K14">
+      <c r="J14" s="4">
         <v>12325.99975585938</v>
       </c>
+      <c r="K14" s="4">
+        <v>8433.599853515625</v>
+      </c>
       <c r="L14">
-        <v>8433.599853515625</v>
-      </c>
-      <c r="M14">
         <v>3295.1998901367192</v>
       </c>
-      <c r="N14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
         <v>46</v>
       </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>47</v>
       </c>
-      <c r="E15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15">
-        <v>161</v>
-      </c>
-      <c r="G15">
+      <c r="F15" s="4">
         <v>2028.600061416626</v>
       </c>
-      <c r="H15">
+      <c r="G15" s="4">
         <v>2746.6599140167241</v>
       </c>
-      <c r="I15">
+      <c r="H15" s="4">
         <v>3620.889963150024</v>
       </c>
-      <c r="J15">
+      <c r="I15" s="4">
         <v>2659.7200736999512</v>
       </c>
-      <c r="K15">
+      <c r="J15" s="4">
         <v>4194.049877166748</v>
       </c>
+      <c r="K15" s="4">
+        <v>2819.110036849976</v>
+      </c>
       <c r="L15">
-        <v>2819.110036849976</v>
-      </c>
-      <c r="M15">
         <v>2291.0299263000488</v>
       </c>
-      <c r="N15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16">
-        <v>25</v>
-      </c>
-      <c r="G16">
+        <v>14</v>
+      </c>
+      <c r="F16" s="5">
         <v>5183.7501525878906</v>
       </c>
-      <c r="H16">
+      <c r="G16" s="4">
         <v>5431.25</v>
       </c>
-      <c r="I16">
+      <c r="H16" s="4">
         <v>5499.2500305175781</v>
       </c>
-      <c r="J16">
+      <c r="I16" s="4">
         <v>5278.2352447509766</v>
       </c>
-      <c r="K16">
+      <c r="J16" s="4">
         <v>5407.4867248535156</v>
       </c>
+      <c r="K16" s="4">
+        <v>4503.9207458496094</v>
+      </c>
       <c r="L16">
-        <v>4503.9207458496094</v>
-      </c>
-      <c r="M16">
         <v>5094.9462890625</v>
       </c>
-      <c r="N16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
         <v>50</v>
       </c>
-      <c r="C17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" t="s">
-        <v>51</v>
-      </c>
       <c r="E17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17">
-        <v>59</v>
-      </c>
-      <c r="G17">
+        <v>22</v>
+      </c>
+      <c r="F17" s="4">
         <v>13814.25996398926</v>
       </c>
-      <c r="H17">
+      <c r="G17" s="4">
         <v>14744.64970397949</v>
       </c>
-      <c r="I17">
+      <c r="H17" s="4">
         <v>13919.185363769529</v>
       </c>
-      <c r="J17">
+      <c r="I17" s="4">
         <v>13493.785064697269</v>
       </c>
-      <c r="K17">
+      <c r="J17" s="4">
         <v>12909.993316650391</v>
       </c>
+      <c r="K17" s="4">
+        <v>12106.905151367189</v>
+      </c>
       <c r="L17">
-        <v>12106.905151367189</v>
-      </c>
-      <c r="M17">
         <v>10351.015060424799</v>
       </c>
-      <c r="N17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18">
-        <v>12</v>
-      </c>
-      <c r="G18">
+        <v>22</v>
+      </c>
+      <c r="F18" s="5">
         <v>4095.599853515625</v>
       </c>
-      <c r="H18">
+      <c r="G18" s="4">
         <v>4477.68017578125</v>
       </c>
-      <c r="I18">
+      <c r="H18" s="4">
         <v>4480.7999267578116</v>
       </c>
-      <c r="J18">
+      <c r="I18" s="4">
         <v>3855.359985351562</v>
       </c>
-      <c r="K18">
+      <c r="J18" s="4">
         <v>4622.7601318359384</v>
       </c>
+      <c r="K18" s="4">
+        <v>3387.359985351562</v>
+      </c>
       <c r="L18">
-        <v>3387.359985351562</v>
-      </c>
-      <c r="M18">
         <v>1101.1200256347661</v>
       </c>
-      <c r="N18" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19">
-        <v>64</v>
-      </c>
-      <c r="G19">
+        <v>22</v>
+      </c>
+      <c r="F19" s="5">
         <v>14053.1201171875</v>
       </c>
-      <c r="H19">
+      <c r="G19" s="4">
         <v>12348.16015625</v>
       </c>
-      <c r="I19">
+      <c r="H19" s="4">
         <v>12291.51953125</v>
       </c>
-      <c r="J19">
+      <c r="I19" s="4">
         <v>10012.2646484375</v>
       </c>
-      <c r="K19">
+      <c r="J19" s="4">
         <v>9274.033203125</v>
       </c>
+      <c r="K19" s="4">
+        <v>8131.4501953125</v>
+      </c>
       <c r="L19">
-        <v>8131.4501953125</v>
-      </c>
-      <c r="M19">
         <v>2636.764404296875</v>
       </c>
-      <c r="N19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
         <v>54</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>55</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>56</v>
       </c>
-      <c r="E20" t="s">
-        <v>57</v>
-      </c>
-      <c r="F20">
-        <v>7</v>
-      </c>
-      <c r="G20">
+      <c r="F20" s="4">
         <v>2810.1500854492192</v>
       </c>
-      <c r="H20">
+      <c r="G20" s="4">
         <v>2631.2999572753911</v>
       </c>
-      <c r="I20">
+      <c r="H20" s="4">
         <v>2581.25</v>
       </c>
-      <c r="J20">
+      <c r="I20" s="4">
         <v>2542.981567382812</v>
       </c>
-      <c r="K20">
+      <c r="J20" s="4">
         <v>2297.66455078125</v>
       </c>
+      <c r="K20" s="4">
+        <v>1424.400344848633</v>
+      </c>
       <c r="L20">
-        <v>1424.400344848633</v>
-      </c>
-      <c r="M20">
         <v>1338.769226074219</v>
       </c>
-      <c r="N20" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
         <v>58</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>59</v>
       </c>
-      <c r="D21" t="s">
-        <v>60</v>
-      </c>
       <c r="E21" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21">
-        <v>12</v>
-      </c>
-      <c r="G21">
+        <v>56</v>
+      </c>
+      <c r="F21" s="4">
         <v>2336.159912109375</v>
       </c>
-      <c r="H21">
+      <c r="G21" s="4">
         <v>2401.7063598632808</v>
       </c>
-      <c r="I21">
+      <c r="H21" s="4">
         <v>2301.55078125</v>
       </c>
-      <c r="J21">
+      <c r="I21" s="4">
         <v>2402.1828002929692</v>
       </c>
-      <c r="K21">
+      <c r="J21" s="4">
         <v>2099.9588012695308</v>
       </c>
+      <c r="K21" s="4">
+        <v>1901.021118164062</v>
+      </c>
       <c r="L21">
-        <v>1901.021118164062</v>
-      </c>
-      <c r="M21">
         <v>1749.717041015625</v>
       </c>
-      <c r="N21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" t="s">
         <v>61</v>
       </c>
-      <c r="C22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" t="s">
-        <v>63</v>
-      </c>
       <c r="E22" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22">
-        <v>13</v>
-      </c>
-      <c r="G22">
+        <v>56</v>
+      </c>
+      <c r="F22" s="4">
         <v>1955.849960327148</v>
       </c>
-      <c r="H22">
+      <c r="G22" s="4">
         <v>1847.3919219970701</v>
       </c>
-      <c r="I22">
+      <c r="H22" s="4">
         <v>1773.3044586181641</v>
       </c>
-      <c r="J22">
+      <c r="I22" s="4">
         <v>1843.635498046875</v>
       </c>
-      <c r="K22">
+      <c r="J22" s="4">
         <v>1711.4858245849609</v>
       </c>
+      <c r="K22" s="4">
+        <v>1681.186080932617</v>
+      </c>
       <c r="L22">
-        <v>1681.186080932617</v>
-      </c>
-      <c r="M22">
         <v>1408.905944824219</v>
       </c>
-      <c r="N22" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" t="s">
         <v>64</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E23" t="s">
         <v>65</v>
       </c>
-      <c r="D23" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23">
-        <v>32</v>
-      </c>
-      <c r="G23">
+      <c r="F23" s="4">
         <v>1757.119995117188</v>
       </c>
-      <c r="H23">
+      <c r="G23" s="4">
         <v>1843.457885742188</v>
       </c>
-      <c r="I23">
+      <c r="H23" s="4">
         <v>2033.856079101562</v>
       </c>
-      <c r="J23">
+      <c r="I23" s="4">
         <v>1836.522827148438</v>
       </c>
-      <c r="K23">
+      <c r="J23" s="4">
         <v>1761.68310546875</v>
       </c>
+      <c r="K23" s="4">
+        <v>1259.49365234375</v>
+      </c>
       <c r="L23">
-        <v>1259.49365234375</v>
-      </c>
-      <c r="M23">
         <v>1896.734008789062</v>
       </c>
-      <c r="N23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E24" t="s">
-        <v>57</v>
-      </c>
-      <c r="F24">
-        <v>21</v>
-      </c>
-      <c r="G24">
+        <v>56</v>
+      </c>
+      <c r="F24" s="4">
         <v>1548.1200256347661</v>
       </c>
-      <c r="H24">
+      <c r="G24" s="4">
         <v>1561.3160018920901</v>
       </c>
-      <c r="I24">
+      <c r="H24" s="4">
         <v>1597.9176406860349</v>
       </c>
-      <c r="J24">
+      <c r="I24" s="4">
         <v>1738.0603408813481</v>
       </c>
-      <c r="K24">
+      <c r="J24" s="4">
         <v>1487.389823913574</v>
       </c>
+      <c r="K24" s="4">
+        <v>1175.033569335938</v>
+      </c>
       <c r="L24">
-        <v>1175.033569335938</v>
-      </c>
-      <c r="M24">
         <v>1297.738700866699</v>
       </c>
-      <c r="N24" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" t="s">
         <v>70</v>
       </c>
-      <c r="C25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" t="s">
-        <v>72</v>
-      </c>
       <c r="E25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25">
-        <v>17</v>
-      </c>
-      <c r="G25">
+        <v>18</v>
+      </c>
+      <c r="F25" s="4">
         <v>1434.800025939941</v>
       </c>
-      <c r="H25">
+      <c r="G25" s="4">
         <v>1307.4700622558589</v>
       </c>
-      <c r="I25">
+      <c r="H25" s="4">
         <v>1238.959953308105</v>
       </c>
-      <c r="J25">
+      <c r="I25" s="4">
         <v>1240.7316513061519</v>
       </c>
-      <c r="K25">
+      <c r="J25" s="4">
         <v>1240.8162155151369</v>
       </c>
+      <c r="K25" s="4">
+        <v>1177.139755249023</v>
+      </c>
       <c r="L25">
-        <v>1177.139755249023</v>
-      </c>
-      <c r="M25">
         <v>911.43414688110352</v>
       </c>
-      <c r="N25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" t="s">
         <v>73</v>
       </c>
-      <c r="C26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" t="s">
-        <v>75</v>
-      </c>
       <c r="E26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26">
-        <v>4</v>
-      </c>
-      <c r="G26">
+        <v>18</v>
+      </c>
+      <c r="F26" s="4">
         <v>1154.0400390625</v>
       </c>
-      <c r="H26">
+      <c r="G26" s="4">
         <v>1138.43994140625</v>
       </c>
-      <c r="I26">
+      <c r="H26" s="4">
         <v>1056.599975585938</v>
       </c>
-      <c r="J26">
+      <c r="I26" s="4">
         <v>1008.650817871094</v>
       </c>
-      <c r="K26">
+      <c r="J26" s="4">
         <v>890.21990966796875</v>
       </c>
+      <c r="K26" s="4">
+        <v>961.9659423828125</v>
+      </c>
       <c r="L26">
-        <v>961.9659423828125</v>
-      </c>
-      <c r="M26">
         <v>886.4459228515625</v>
       </c>
-      <c r="N26" t="s">
-        <v>101</v>
-      </c>
+      <c r="M26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Formatting changes to spreadsheets, heatmap choice of colour scheme dropdown
</commit_message>
<xml_diff>
--- a/assets/Historical Performance.xlsx
+++ b/assets/Historical Performance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard\PycharmProjects\dash\YT_Dash_Tutorial\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardwalker/PycharmProjects/Dash_Equity/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7D3A27-DD8C-46AC-A14C-4AD9A340E069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E824770-8463-174B-B1A8-C24818182489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="240" windowWidth="29040" windowHeight="16455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25980" windowHeight="12680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -341,8 +341,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -410,7 +410,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -421,8 +421,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -728,20 +728,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -779,7 +778,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -820,7 +819,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -861,7 +860,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -902,7 +901,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -943,7 +942,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -984,7 +983,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1013,7 +1012,7 @@
         <v>4579.0799865722656</v>
       </c>
       <c r="J7" s="4">
-        <v>5481.5200805664063</v>
+        <v>5481.5200805664062</v>
       </c>
       <c r="K7" s="4">
         <v>3295.1599731445308</v>
@@ -1025,7 +1024,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1066,7 +1065,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1107,7 +1106,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1148,7 +1147,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1189,7 +1188,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1230,7 +1229,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1271,7 +1270,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1312,7 +1311,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1353,7 +1352,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1394,7 +1393,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1435,7 +1434,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1476,7 +1475,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1517,7 +1516,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1558,7 +1557,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1599,7 +1598,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1640,7 +1639,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1681,7 +1680,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1722,7 +1721,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1763,7 +1762,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1804,7 +1803,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -1812,7 +1811,7 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>

</xml_diff>